<commit_message>
documentation added to syssettings and scenario files
</commit_message>
<xml_diff>
--- a/TIMES-NZ/SysSettings.xlsx
+++ b/TIMES-NZ/SysSettings.xlsx
@@ -1,28 +1,29 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rbsul\Documents\GitHub\TIMES-NZ-Model-Files\TIMES-NZ\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greeda\git\TIMES-NZ-Model-Files\TIMES-NZ\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FC67264-AA47-47D2-9796-F1D1C9B5727E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60E78621-0917-4637-9CE3-C11D9069C380}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" tabRatio="853" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5025" yWindow="-18120" windowWidth="29040" windowHeight="17520" tabRatio="853" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Region-Time Slices" sheetId="16" r:id="rId1"/>
-    <sheet name="TimePeriods" sheetId="18" r:id="rId2"/>
-    <sheet name="Import Settings" sheetId="17" r:id="rId3"/>
-    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" r:id="rId4"/>
-    <sheet name="Constants" sheetId="20" r:id="rId5"/>
-    <sheet name="Commodity Group" sheetId="15" r:id="rId6"/>
-    <sheet name="Defaults" sheetId="21" r:id="rId7"/>
+    <sheet name="Documentation" sheetId="22" r:id="rId1"/>
+    <sheet name="Region-Time Slices" sheetId="16" r:id="rId2"/>
+    <sheet name="TimePeriods" sheetId="18" r:id="rId3"/>
+    <sheet name="Import Settings" sheetId="17" r:id="rId4"/>
+    <sheet name="Interpol_Extrapol_Defaults" sheetId="14" r:id="rId5"/>
+    <sheet name="Constants" sheetId="20" r:id="rId6"/>
+    <sheet name="Commodity Group" sheetId="15" r:id="rId7"/>
+    <sheet name="Defaults" sheetId="21" r:id="rId8"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId8"/>
+    <externalReference r:id="rId9"/>
   </externalReferences>
   <definedNames>
     <definedName name="FID_1">[1]AGR_Fuels!$A$2</definedName>
@@ -128,7 +129,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="365" uniqueCount="171">
   <si>
     <t>IMP*Z</t>
   </si>
@@ -618,6 +619,30 @@
   <si>
     <t>~TFM_INS-TXT</t>
   </si>
+  <si>
+    <t>Workbook: Base settings for TIMES model</t>
+  </si>
+  <si>
+    <t>Region-Time Slices: Timeslice definitions</t>
+  </si>
+  <si>
+    <t>TimePeriods: Set number and length of model time periods</t>
+  </si>
+  <si>
+    <t>Import Settings: Base run settings</t>
+  </si>
+  <si>
+    <t>Interpol_Extrapol_Defaults: Interpolation and Extrapolation settings</t>
+  </si>
+  <si>
+    <t>Constants: Discount rate and timeslice length</t>
+  </si>
+  <si>
+    <t>Commodity Group: Commodity group defintions</t>
+  </si>
+  <si>
+    <t>Defaults: Default units</t>
+  </si>
 </sst>
 </file>
 
@@ -629,7 +654,7 @@
     <numFmt numFmtId="166" formatCode="0.0000"/>
     <numFmt numFmtId="167" formatCode="_-[$€-2]* #,##0.00_-;\-[$€-2]* #,##0.00_-;_-[$€-2]* &quot;-&quot;??_-"/>
   </numFmts>
-  <fonts count="62">
+  <fonts count="62" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -16222,6 +16247,61 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F8D1A57-CDAE-4682-907E-2EE2CABFDB12}">
+  <dimension ref="A1:A8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G8"/>
   <sheetViews>
@@ -16229,17 +16309,17 @@
       <selection activeCell="C8" sqref="B7:C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="7" width="13.81640625" style="24" customWidth="1"/>
+    <col min="1" max="7" width="13.85546875" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="32" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="13">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="s">
         <v>7</v>
       </c>
@@ -16249,7 +16329,7 @@
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
     </row>
-    <row r="4" spans="1:7" ht="13">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B4" s="21" t="s">
         <v>13</v>
       </c>
@@ -16266,7 +16346,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B5" s="18" t="s">
         <v>66</v>
       </c>
@@ -16283,7 +16363,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="B6" s="18" t="s">
         <v>67</v>
       </c>
@@ -16300,7 +16380,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E7" s="23" t="s">
         <v>70</v>
       </c>
@@ -16309,7 +16389,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="E8" s="23" t="s">
         <v>71</v>
       </c>
@@ -16325,7 +16405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:E24"/>
   <sheetViews>
@@ -16333,39 +16413,39 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="4" width="10" customWidth="1"/>
-    <col min="5" max="5" width="17.81640625" customWidth="1"/>
-    <col min="6" max="8" width="8.453125" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" customWidth="1"/>
+    <col min="6" max="8" width="8.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:5">
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="2:5">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4">
         <v>2018</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="11" spans="2:5">
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B12" s="34" t="s">
         <v>151</v>
       </c>
@@ -16379,7 +16459,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B13" s="27">
         <v>1</v>
       </c>
@@ -16393,7 +16473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B14" s="27">
         <v>2</v>
       </c>
@@ -16407,7 +16487,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B15" s="27">
         <v>5</v>
       </c>
@@ -16421,7 +16501,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B16" s="27">
         <v>5</v>
       </c>
@@ -16435,7 +16515,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="2:5">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B17" s="27">
         <v>5</v>
       </c>
@@ -16449,7 +16529,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="2:5">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B18" s="27">
         <v>5</v>
       </c>
@@ -16463,7 +16543,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="2:5">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B19" s="27">
         <v>5</v>
       </c>
@@ -16477,7 +16557,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="2:5">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B20" s="27">
         <v>5</v>
       </c>
@@ -16491,7 +16571,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="2:5">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B21" s="27">
         <v>5</v>
       </c>
@@ -16505,7 +16585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:5">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B22" s="27">
         <v>5</v>
       </c>
@@ -16519,7 +16599,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="2:5">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B23" s="27">
         <v>5</v>
       </c>
@@ -16531,7 +16611,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="2:5">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B24" s="27"/>
       <c r="C24" s="27">
         <v>5</v>
@@ -16549,7 +16629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:C10"/>
   <sheetViews>
@@ -16557,18 +16637,18 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.453125" customWidth="1"/>
-    <col min="2" max="2" width="52.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.42578125" customWidth="1"/>
+    <col min="2" max="2" width="52.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" ht="13">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="26" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="2:3" ht="13">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="28" t="s">
         <v>30</v>
       </c>
@@ -16576,7 +16656,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="2:3">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="29" t="s">
         <v>32</v>
       </c>
@@ -16584,7 +16664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="29" t="s">
         <v>33</v>
       </c>
@@ -16592,7 +16672,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:3">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="29" t="s">
         <v>34</v>
       </c>
@@ -16600,7 +16680,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="29" t="s">
         <v>35</v>
       </c>
@@ -16608,7 +16688,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="29" t="s">
         <v>74</v>
       </c>
@@ -16616,7 +16696,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="29" t="s">
         <v>57</v>
       </c>
@@ -16632,40 +16712,40 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.81640625" style="24" customWidth="1"/>
-    <col min="2" max="3" width="9.1796875" style="24"/>
-    <col min="4" max="4" width="9.7265625" style="24" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.7265625" style="24" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1796875" style="24" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.7265625" style="24" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="10.7265625" style="24" customWidth="1"/>
-    <col min="10" max="12" width="9.1796875" style="24"/>
-    <col min="13" max="13" width="9.26953125" style="24" customWidth="1"/>
-    <col min="14" max="16384" width="9.1796875" style="24"/>
+    <col min="1" max="1" width="2.85546875" style="24" customWidth="1"/>
+    <col min="2" max="3" width="9.140625" style="24"/>
+    <col min="4" max="4" width="9.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.140625" style="24" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="10.7109375" style="24" customWidth="1"/>
+    <col min="10" max="12" width="9.140625" style="24"/>
+    <col min="13" max="13" width="9.28515625" style="24" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="24">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="13">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B3" s="19" t="str">
         <f>IF($A$1=1,"~TFM_MIG","~TFM_UPD")</f>
         <v>~TFM_MIG</v>
       </c>
     </row>
-    <row r="4" spans="1:17">
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B4" s="20" t="s">
         <v>17</v>
       </c>
@@ -16707,7 +16787,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:17">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B5" s="23"/>
       <c r="C5" s="18" t="s">
         <v>75</v>
@@ -16732,7 +16812,7 @@
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
     </row>
-    <row r="6" spans="1:17">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B6" s="23"/>
       <c r="C6" s="18" t="s">
         <v>75</v>
@@ -16759,7 +16839,7 @@
       <c r="M6" s="23"/>
       <c r="N6" s="23"/>
     </row>
-    <row r="7" spans="1:17">
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B7" s="23"/>
       <c r="C7" s="18" t="s">
         <v>75</v>
@@ -16786,7 +16866,7 @@
       <c r="M7" s="23"/>
       <c r="N7" s="23"/>
     </row>
-    <row r="8" spans="1:17">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B8" s="23" t="s">
         <v>149</v>
       </c>
@@ -16813,7 +16893,7 @@
       <c r="M8" s="23"/>
       <c r="N8" s="23"/>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B9" s="23" t="s">
         <v>149</v>
       </c>
@@ -16840,7 +16920,7 @@
       <c r="M9" s="23"/>
       <c r="N9" s="23"/>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B10" s="23"/>
       <c r="C10" s="18" t="s">
         <v>75</v>
@@ -16867,17 +16947,17 @@
       <c r="M10" s="23"/>
       <c r="N10" s="23"/>
     </row>
-    <row r="11" spans="1:17" ht="17.5">
+    <row r="11" spans="1:17" ht="18" x14ac:dyDescent="0.25">
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
     </row>
-    <row r="13" spans="1:17" ht="13">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B14" s="20" t="s">
         <v>17</v>
       </c>
@@ -16927,7 +17007,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
       <c r="D15" s="23" t="s">
@@ -16953,7 +17033,7 @@
       <c r="P15" s="23"/>
       <c r="Q15" s="23"/>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
       <c r="D16" s="23" t="s">
@@ -16979,12 +17059,12 @@
       <c r="P16" s="23"/>
       <c r="Q16" s="23"/>
     </row>
-    <row r="21" spans="2:17" ht="13">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B21" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="2:17">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B22" s="20" t="s">
         <v>17</v>
       </c>
@@ -17034,7 +17114,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="2:17">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B23" s="23"/>
       <c r="C23" s="23" t="s">
         <v>150</v>
@@ -17062,7 +17142,7 @@
       <c r="P23" s="23"/>
       <c r="Q23" s="23"/>
     </row>
-    <row r="24" spans="2:17">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B24" s="23"/>
       <c r="C24" s="23" t="s">
         <v>150</v>
@@ -17090,7 +17170,7 @@
       <c r="P24" s="23"/>
       <c r="Q24" s="23"/>
     </row>
-    <row r="25" spans="2:17">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B25" s="23"/>
       <c r="D25" s="23" t="s">
         <v>58</v>
@@ -17111,7 +17191,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="2:17">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B26" s="23"/>
       <c r="C26" s="23"/>
       <c r="D26" s="23"/>
@@ -17123,7 +17203,7 @@
       <c r="J26" s="23"/>
       <c r="K26" s="23"/>
     </row>
-    <row r="27" spans="2:17">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B27" s="33"/>
       <c r="D27" s="33"/>
       <c r="E27" s="33"/>
@@ -17134,7 +17214,7 @@
       <c r="J27" s="33"/>
       <c r="K27" s="33"/>
     </row>
-    <row r="28" spans="2:17">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B28" s="33"/>
       <c r="D28" s="33"/>
       <c r="E28" s="33"/>
@@ -17145,12 +17225,12 @@
       <c r="J28" s="33"/>
       <c r="K28" s="33"/>
     </row>
-    <row r="30" spans="2:17" ht="13">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B30" s="2" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="31" spans="2:17">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B31" s="20" t="s">
         <v>17</v>
       </c>
@@ -17200,7 +17280,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="32" spans="2:17">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.2">
       <c r="B32" s="23"/>
       <c r="C32" s="23"/>
       <c r="D32" s="23" t="s">
@@ -17234,7 +17314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B4:K63"/>
   <sheetViews>
@@ -17242,24 +17322,24 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="3"/>
-    <col min="2" max="2" width="23.26953125" style="3" customWidth="1"/>
-    <col min="3" max="4" width="12.453125" style="3" customWidth="1"/>
-    <col min="5" max="5" width="10.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.453125" style="3" customWidth="1"/>
-    <col min="7" max="8" width="9.1796875" style="3"/>
-    <col min="9" max="9" width="11.1796875" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="3"/>
+    <col min="1" max="1" width="9.140625" style="3"/>
+    <col min="2" max="2" width="23.28515625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="12.42578125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" style="3" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="3"/>
+    <col min="9" max="9" width="11.140625" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:8" ht="13">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="2:8">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B5" s="20" t="s">
         <v>17</v>
       </c>
@@ -17282,7 +17362,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="2:8">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B6" s="13"/>
       <c r="C6" s="13"/>
       <c r="D6" s="13" t="s">
@@ -17295,7 +17375,7 @@
       <c r="G6" s="13"/>
       <c r="H6" s="13"/>
     </row>
-    <row r="7" spans="2:8">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B7" s="13"/>
       <c r="C7" s="13"/>
       <c r="D7" s="13" t="s">
@@ -17308,7 +17388,7 @@
       <c r="G7" s="13"/>
       <c r="H7" s="13"/>
     </row>
-    <row r="8" spans="2:8">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="13" t="s">
         <v>77</v>
       </c>
@@ -17324,7 +17404,7 @@
       <c r="G8" s="13"/>
       <c r="H8" s="13"/>
     </row>
-    <row r="9" spans="2:8">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
         <v>78</v>
       </c>
@@ -17340,7 +17420,7 @@
       <c r="G9" s="13"/>
       <c r="H9" s="13"/>
     </row>
-    <row r="10" spans="2:8">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
         <v>135</v>
       </c>
@@ -17356,7 +17436,7 @@
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>
     </row>
-    <row r="11" spans="2:8">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="13" t="s">
         <v>79</v>
       </c>
@@ -17372,7 +17452,7 @@
       <c r="G11" s="13"/>
       <c r="H11" s="13"/>
     </row>
-    <row r="12" spans="2:8">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="13" t="s">
         <v>80</v>
       </c>
@@ -17388,7 +17468,7 @@
       <c r="G12" s="13"/>
       <c r="H12" s="13"/>
     </row>
-    <row r="13" spans="2:8">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B13" s="13" t="s">
         <v>137</v>
       </c>
@@ -17404,7 +17484,7 @@
       <c r="G13" s="12"/>
       <c r="H13" s="13"/>
     </row>
-    <row r="14" spans="2:8">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="13" t="s">
         <v>81</v>
       </c>
@@ -17420,7 +17500,7 @@
       <c r="G14" s="12"/>
       <c r="H14" s="13"/>
     </row>
-    <row r="15" spans="2:8">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B15" s="13" t="s">
         <v>82</v>
       </c>
@@ -17436,7 +17516,7 @@
       <c r="G15" s="12"/>
       <c r="H15" s="13"/>
     </row>
-    <row r="16" spans="2:8">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="13" t="s">
         <v>138</v>
       </c>
@@ -17452,7 +17532,7 @@
       <c r="G16" s="12"/>
       <c r="H16" s="13"/>
     </row>
-    <row r="17" spans="2:8">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="13" t="s">
         <v>83</v>
       </c>
@@ -17468,7 +17548,7 @@
       <c r="G17" s="12"/>
       <c r="H17" s="13"/>
     </row>
-    <row r="18" spans="2:8">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="13" t="s">
         <v>84</v>
       </c>
@@ -17484,7 +17564,7 @@
       <c r="G18" s="12"/>
       <c r="H18" s="13"/>
     </row>
-    <row r="19" spans="2:8">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="13" t="s">
         <v>139</v>
       </c>
@@ -17500,7 +17580,7 @@
       <c r="G19" s="12"/>
       <c r="H19" s="13"/>
     </row>
-    <row r="20" spans="2:8">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>85</v>
       </c>
@@ -17516,7 +17596,7 @@
       <c r="G20" s="12"/>
       <c r="H20" s="13"/>
     </row>
-    <row r="21" spans="2:8">
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="13" t="s">
         <v>86</v>
       </c>
@@ -17532,7 +17612,7 @@
       <c r="G21" s="13"/>
       <c r="H21" s="13"/>
     </row>
-    <row r="22" spans="2:8">
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="13" t="s">
         <v>140</v>
       </c>
@@ -17548,7 +17628,7 @@
       <c r="G22" s="13"/>
       <c r="H22" s="13"/>
     </row>
-    <row r="23" spans="2:8">
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="13" t="s">
         <v>87</v>
       </c>
@@ -17564,7 +17644,7 @@
       <c r="G23" s="13"/>
       <c r="H23" s="13"/>
     </row>
-    <row r="24" spans="2:8">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="13" t="s">
         <v>88</v>
       </c>
@@ -17580,7 +17660,7 @@
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
     </row>
-    <row r="25" spans="2:8">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B25" s="13" t="s">
         <v>141</v>
       </c>
@@ -17596,7 +17676,7 @@
       <c r="G25" s="13"/>
       <c r="H25" s="13"/>
     </row>
-    <row r="26" spans="2:8">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
         <v>89</v>
       </c>
@@ -17612,7 +17692,7 @@
       <c r="G26" s="13"/>
       <c r="H26" s="13"/>
     </row>
-    <row r="27" spans="2:8">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B27" s="13" t="s">
         <v>90</v>
       </c>
@@ -17628,7 +17708,7 @@
       <c r="G27" s="13"/>
       <c r="H27" s="13"/>
     </row>
-    <row r="28" spans="2:8">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B28" s="13" t="s">
         <v>142</v>
       </c>
@@ -17644,7 +17724,7 @@
       <c r="G28" s="13"/>
       <c r="H28" s="13"/>
     </row>
-    <row r="29" spans="2:8">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
         <v>91</v>
       </c>
@@ -17660,7 +17740,7 @@
       <c r="G29" s="13"/>
       <c r="H29" s="13"/>
     </row>
-    <row r="30" spans="2:8">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B30" s="13" t="s">
         <v>92</v>
       </c>
@@ -17676,7 +17756,7 @@
       <c r="G30" s="13"/>
       <c r="H30" s="13"/>
     </row>
-    <row r="31" spans="2:8">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B31" s="13" t="s">
         <v>143</v>
       </c>
@@ -17692,7 +17772,7 @@
       <c r="G31" s="13"/>
       <c r="H31" s="13"/>
     </row>
-    <row r="32" spans="2:8">
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B32" s="13"/>
       <c r="C32" s="23"/>
       <c r="D32" s="13"/>
@@ -17701,7 +17781,7 @@
       <c r="G32" s="13"/>
       <c r="H32" s="13"/>
     </row>
-    <row r="33" spans="2:11">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B33" s="13"/>
       <c r="C33" s="23"/>
       <c r="D33" s="13" t="s">
@@ -17721,10 +17801,10 @@
         <v>93</v>
       </c>
     </row>
-    <row r="34" spans="2:11">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.2">
       <c r="C34"/>
     </row>
-    <row r="37" spans="2:11">
+    <row r="37" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B37" s="14"/>
       <c r="C37" s="37" t="s">
         <v>94</v>
@@ -17737,7 +17817,7 @@
       <c r="I37" s="14"/>
       <c r="J37" s="14"/>
     </row>
-    <row r="38" spans="2:11">
+    <row r="38" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B38" s="14"/>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
@@ -17754,7 +17834,7 @@
         <v>8.0812535184837664E-2</v>
       </c>
     </row>
-    <row r="39" spans="2:11">
+    <row r="39" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B39" s="39" t="s">
         <v>95</v>
       </c>
@@ -17780,7 +17860,7 @@
         <v>8.8159129292550181E-2</v>
       </c>
     </row>
-    <row r="40" spans="2:11">
+    <row r="40" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B40" s="40"/>
       <c r="C40" s="23"/>
       <c r="D40" s="23"/>
@@ -17804,7 +17884,7 @@
         <v>7.3465941077125148E-3</v>
       </c>
     </row>
-    <row r="41" spans="2:11">
+    <row r="41" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B41" s="40"/>
       <c r="C41" s="23"/>
       <c r="D41" s="23"/>
@@ -17828,7 +17908,7 @@
         <v>3.2201163445299302E-2</v>
       </c>
     </row>
-    <row r="42" spans="2:11">
+    <row r="42" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B42" s="40"/>
       <c r="C42" s="23"/>
       <c r="D42" s="23"/>
@@ -17852,7 +17932,7 @@
         <v>3.512854194032651E-2</v>
       </c>
     </row>
-    <row r="43" spans="2:11">
+    <row r="43" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B43" s="14"/>
       <c r="C43" s="13"/>
       <c r="D43" s="13"/>
@@ -17872,7 +17952,7 @@
         <v>2.9273784950272089E-3</v>
       </c>
     </row>
-    <row r="44" spans="2:11">
+    <row r="44" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B44" s="14"/>
       <c r="C44" s="13"/>
       <c r="D44" s="13"/>
@@ -17889,7 +17969,7 @@
         <v>8.26083693000563E-2</v>
       </c>
     </row>
-    <row r="45" spans="2:11">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B45" s="39" t="s">
         <v>96</v>
       </c>
@@ -17915,7 +17995,7 @@
         <v>9.0118221054606873E-2</v>
       </c>
     </row>
-    <row r="46" spans="2:11">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B46" s="40"/>
       <c r="C46" s="23"/>
       <c r="D46" s="23"/>
@@ -17940,7 +18020,7 @@
         <v>7.5098517545505727E-3</v>
       </c>
     </row>
-    <row r="47" spans="2:11">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B47" s="14"/>
       <c r="C47" s="13"/>
       <c r="D47" s="13"/>
@@ -17957,7 +18037,7 @@
         <v>3.291674485519485E-2</v>
       </c>
     </row>
-    <row r="48" spans="2:11">
+    <row r="48" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B48" s="14"/>
       <c r="C48" s="14" t="s">
         <v>98</v>
@@ -17986,7 +18066,7 @@
         <v>3.5909176205667109E-2</v>
       </c>
     </row>
-    <row r="49" spans="2:11">
+    <row r="49" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B49" s="39" t="s">
         <v>97</v>
       </c>
@@ -18022,7 +18102,7 @@
         <v>2.9924313504722591E-3</v>
       </c>
     </row>
-    <row r="50" spans="2:11">
+    <row r="50" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B50" s="40"/>
       <c r="C50" s="13">
         <v>11</v>
@@ -18056,7 +18136,7 @@
         <v>8.26083693000563E-2</v>
       </c>
     </row>
-    <row r="51" spans="2:11">
+    <row r="51" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B51" s="40"/>
       <c r="C51" s="13">
         <v>11</v>
@@ -18090,7 +18170,7 @@
         <v>9.0118221054606873E-2</v>
       </c>
     </row>
-    <row r="52" spans="2:11">
+    <row r="52" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B52" s="40"/>
       <c r="C52" s="13">
         <v>11</v>
@@ -18124,7 +18204,7 @@
         <v>7.5098517545505727E-3</v>
       </c>
     </row>
-    <row r="53" spans="2:11">
+    <row r="53" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B53" s="14"/>
       <c r="C53" s="13"/>
       <c r="D53" s="13"/>
@@ -18141,7 +18221,7 @@
         <v>3.291674485519485E-2</v>
       </c>
     </row>
-    <row r="54" spans="2:11">
+    <row r="54" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B54" s="11"/>
       <c r="C54" s="22"/>
       <c r="D54" s="22"/>
@@ -18158,7 +18238,7 @@
         <v>3.5909176205667109E-2</v>
       </c>
     </row>
-    <row r="55" spans="2:11">
+    <row r="55" spans="2:11" x14ac:dyDescent="0.2">
       <c r="B55" s="11"/>
       <c r="C55" s="22"/>
       <c r="D55" s="22"/>
@@ -18175,7 +18255,7 @@
         <v>2.9924313504722591E-3</v>
       </c>
     </row>
-    <row r="56" spans="2:11">
+    <row r="56" spans="2:11" x14ac:dyDescent="0.2">
       <c r="J56" s="13" t="s">
         <v>89</v>
       </c>
@@ -18184,7 +18264,7 @@
         <v>8.1710452242446982E-2</v>
       </c>
     </row>
-    <row r="57" spans="2:11">
+    <row r="57" spans="2:11" x14ac:dyDescent="0.2">
       <c r="J57" s="13" t="s">
         <v>90</v>
       </c>
@@ -18193,7 +18273,7 @@
         <v>8.9138675173578527E-2</v>
       </c>
     </row>
-    <row r="58" spans="2:11">
+    <row r="58" spans="2:11" x14ac:dyDescent="0.2">
       <c r="J58" s="13" t="s">
         <v>142</v>
       </c>
@@ -18202,7 +18282,7 @@
         <v>7.4282229311315433E-3</v>
       </c>
     </row>
-    <row r="59" spans="2:11">
+    <row r="59" spans="2:11" x14ac:dyDescent="0.2">
       <c r="J59" s="13" t="s">
         <v>91</v>
       </c>
@@ -18211,7 +18291,7 @@
         <v>3.2558954150247073E-2</v>
       </c>
     </row>
-    <row r="60" spans="2:11">
+    <row r="60" spans="2:11" x14ac:dyDescent="0.2">
       <c r="J60" s="13" t="s">
         <v>92</v>
       </c>
@@ -18220,7 +18300,7 @@
         <v>3.551885907299681E-2</v>
       </c>
     </row>
-    <row r="61" spans="2:11">
+    <row r="61" spans="2:11" x14ac:dyDescent="0.2">
       <c r="J61" s="13" t="s">
         <v>143</v>
       </c>
@@ -18229,7 +18309,7 @@
         <v>2.959904922749734E-3</v>
       </c>
     </row>
-    <row r="63" spans="2:11">
+    <row r="63" spans="2:11" x14ac:dyDescent="0.2">
       <c r="J63" s="22" t="s">
         <v>99</v>
       </c>
@@ -18252,7 +18332,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="B3:I14"/>
   <sheetViews>
@@ -18260,24 +18340,24 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.1796875" customWidth="1"/>
-    <col min="2" max="2" width="15.7265625" customWidth="1"/>
-    <col min="3" max="3" width="32.1796875" customWidth="1"/>
-    <col min="4" max="4" width="8.7265625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.81640625" customWidth="1"/>
-    <col min="6" max="6" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="11.26953125" customWidth="1"/>
-    <col min="9" max="11" width="11.81640625" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.7109375" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.85546875" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="11.28515625" customWidth="1"/>
+    <col min="9" max="11" width="11.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:9" ht="18" customHeight="1">
+    <row r="3" spans="2:9" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B3" s="1" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="4" spans="2:9" ht="18.75" customHeight="1">
+    <row r="4" spans="2:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B4" s="20" t="s">
         <v>5</v>
       </c>
@@ -18303,7 +18383,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="5" spans="2:9" ht="26">
+    <row r="5" spans="2:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B5" s="25" t="s">
         <v>38</v>
       </c>
@@ -18317,7 +18397,7 @@
       <c r="H5" s="25"/>
       <c r="I5" s="25"/>
     </row>
-    <row r="6" spans="2:9">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B6" s="13" t="s">
         <v>105</v>
       </c>
@@ -18341,7 +18421,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="7" spans="2:9">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B7" s="13" t="s">
         <v>108</v>
       </c>
@@ -18365,7 +18445,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="8" spans="2:9">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B8" s="13" t="s">
         <v>111</v>
       </c>
@@ -18389,7 +18469,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="9" spans="2:9">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B9" s="13" t="s">
         <v>114</v>
       </c>
@@ -18413,7 +18493,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="2:9">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B10" s="13" t="s">
         <v>117</v>
       </c>
@@ -18437,7 +18517,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="11" spans="2:9">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B11" s="13" t="s">
         <v>120</v>
       </c>
@@ -18461,7 +18541,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="12" spans="2:9">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B12" s="13" t="s">
         <v>123</v>
       </c>
@@ -18485,7 +18565,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="13" spans="2:9">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B13" s="13" t="s">
         <v>126</v>
       </c>
@@ -18509,7 +18589,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="14" spans="2:9">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
       <c r="B14" s="13" t="s">
         <v>129</v>
       </c>
@@ -18542,7 +18622,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="B2:M6"/>
   <sheetViews>
@@ -18550,17 +18630,17 @@
       <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="12.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.1796875" style="24"/>
-    <col min="2" max="2" width="11.7265625" style="24" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.1796875" style="24"/>
-    <col min="4" max="4" width="15.54296875" style="24" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="24"/>
+    <col min="2" max="2" width="11.7109375" style="24" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" style="24"/>
+    <col min="4" max="4" width="15.5703125" style="24" bestFit="1" customWidth="1"/>
     <col min="5" max="9" width="10" style="24" customWidth="1"/>
-    <col min="10" max="16384" width="9.1796875" style="24"/>
+    <col min="10" max="16384" width="9.140625" style="24"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:13" ht="13">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" s="19" t="s">
         <v>41</v>
       </c>
@@ -18568,7 +18648,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="2:13">
+    <row r="3" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B3" s="7" t="s">
         <v>42</v>
       </c>
@@ -18591,7 +18671,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="4" spans="2:13">
+    <row r="4" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B4" s="18" t="s">
         <v>100</v>
       </c>
@@ -18620,7 +18700,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="5" spans="2:13">
+    <row r="5" spans="2:13" x14ac:dyDescent="0.2">
       <c r="D5" s="23" t="s">
         <v>45</v>
       </c>
@@ -18646,7 +18726,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="6" spans="2:13">
+    <row r="6" spans="2:13" x14ac:dyDescent="0.2">
       <c r="D6" s="23" t="s">
         <v>46</v>
       </c>

</xml_diff>